<commit_message>
Dataset update + ARMA add
</commit_message>
<xml_diff>
--- a/data/feature_ranking.xlsx
+++ b/data/feature_ranking.xlsx
@@ -756,22 +756,22 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.02996950436575307</v>
+        <v>0.0374236543723061</v>
       </c>
       <c r="C2">
-        <v>0.109813095849202</v>
+        <v>0.1179353445312053</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>-0.03346339470561963</v>
+        <v>-0.03266871208437346</v>
       </c>
       <c r="F2">
         <v>-0</v>
       </c>
       <c r="G2">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -779,22 +779,22 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.582808199761407</v>
+        <v>0.5812209723224382</v>
       </c>
       <c r="C3">
-        <v>0.001399908820572675</v>
+        <v>0.001464884192193381</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.2685375208286064</v>
+        <v>0.2673395661147749</v>
       </c>
       <c r="F3">
-        <v>-1.404982629623968e-07</v>
+        <v>-1.404306763969208e-07</v>
       </c>
       <c r="G3">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -802,19 +802,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.6351677087825096</v>
+        <v>0.6339648224911052</v>
       </c>
       <c r="C4">
-        <v>3.892292268943805e-13</v>
+        <v>5.246455736176005e-13</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.3703590049157746</v>
+        <v>0.3687317004244231</v>
       </c>
       <c r="F4">
-        <v>1.486670704686221e-05</v>
+        <v>1.466268513798869e-05</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -825,22 +825,22 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.6098191706993354</v>
+        <v>0.6090973162027979</v>
       </c>
       <c r="C5">
-        <v>6.662030818159622e-12</v>
+        <v>8.614687966824771e-12</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0.3011682736995294</v>
+        <v>0.2995927775737754</v>
       </c>
       <c r="F5">
-        <v>8.278467845280953e-06</v>
+        <v>8.453655999657912e-06</v>
       </c>
       <c r="G5">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -848,19 +848,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.2898795963446381</v>
+        <v>0.2994378211465327</v>
       </c>
       <c r="C6">
-        <v>4.801913777211936e-47</v>
+        <v>1.578384229301156e-46</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.3742024583674611</v>
+        <v>0.3728699759610937</v>
       </c>
       <c r="G6">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -868,19 +868,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.08976239568772248</v>
+        <v>0.09395066229040072</v>
       </c>
       <c r="C7">
-        <v>0.0001887500225852734</v>
+        <v>0.0002361645955944411</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <v>0.2638145283133759</v>
+        <v>0.2623647948211957</v>
       </c>
       <c r="F7">
-        <v>-1.915756640861426e-05</v>
+        <v>-1.940736600451707e-05</v>
       </c>
       <c r="G7">
         <v>14</v>
@@ -891,22 +891,22 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.6092257077859493</v>
+        <v>0.6165729079999527</v>
       </c>
       <c r="C8">
-        <v>1.727603964619233e-09</v>
+        <v>1.747229789610688e-09</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>0.2648113202482231</v>
+        <v>0.2634580759630122</v>
       </c>
       <c r="F8">
-        <v>-3.838822090289126e-07</v>
+        <v>-3.442000223503434e-07</v>
       </c>
       <c r="G8">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -914,22 +914,22 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>0.5336600029312</v>
+        <v>0.5391119072762223</v>
       </c>
       <c r="C9">
-        <v>2.045674929137632e-05</v>
+        <v>2.882494835657383e-05</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>0.123831555355631</v>
+        <v>0.1226055883417212</v>
       </c>
       <c r="F9">
-        <v>-1.063840634521192e-06</v>
+        <v>-1.071332123355441e-06</v>
       </c>
       <c r="G9">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -937,22 +937,22 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>0.6001542033654061</v>
+        <v>0.6013542443317479</v>
       </c>
       <c r="C10">
-        <v>1.86961643207628e-13</v>
+        <v>3.058156464744496e-13</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>0.2975835158912593</v>
+        <v>0.2964252283225013</v>
       </c>
       <c r="F10">
-        <v>3.198892542883371e-07</v>
+        <v>3.013312542900627e-07</v>
       </c>
       <c r="G10">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -960,22 +960,22 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>0.5738553608067001</v>
+        <v>0.5754108130510152</v>
       </c>
       <c r="C11">
-        <v>0.0004072709351223214</v>
+        <v>0.0004079994237843811</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>0.2060899157976127</v>
+        <v>0.2051287964746347</v>
       </c>
       <c r="F11">
-        <v>2.774921702173113e-07</v>
+        <v>2.802129212704315e-07</v>
       </c>
       <c r="G11">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -983,22 +983,22 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>0.5527402497017566</v>
+        <v>0.5529566636951144</v>
       </c>
       <c r="C12">
-        <v>0.3604253085997781</v>
+        <v>0.3587431923219093</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0.1849889690395231</v>
+        <v>0.1840693737575493</v>
       </c>
       <c r="F12">
-        <v>-1.529354963833542e-08</v>
+        <v>-1.503894914538964e-08</v>
       </c>
       <c r="G12">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1006,22 +1006,22 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>0.5658790317581119</v>
+        <v>0.5713837979721932</v>
       </c>
       <c r="C13">
-        <v>6.068140348795631e-14</v>
+        <v>9.61830587173709e-14</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>0.2282045935858485</v>
+        <v>0.2269661071489471</v>
       </c>
       <c r="F13">
-        <v>8.7158295689545e-06</v>
+        <v>8.546785978107374e-06</v>
       </c>
       <c r="G13">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1029,22 +1029,22 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>0.5767660343302987</v>
+        <v>0.5732011378633537</v>
       </c>
       <c r="C14">
-        <v>1.401623391819938e-10</v>
+        <v>1.963957919428311e-10</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>0.3061263735090292</v>
+        <v>0.3049564811538901</v>
       </c>
       <c r="F14">
-        <v>-2.063416161998574e-07</v>
+        <v>-2.057507916181049e-07</v>
       </c>
       <c r="G14">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1052,22 +1052,22 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>0.5597656696585247</v>
+        <v>0.560822108086624</v>
       </c>
       <c r="C15">
-        <v>4.405424839184405e-07</v>
+        <v>5.317844682325863e-07</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>0.2640459087877899</v>
+        <v>0.2628222066800103</v>
       </c>
       <c r="F15">
-        <v>2.57023064921675e-06</v>
+        <v>2.549059829875582e-06</v>
       </c>
       <c r="G15">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1075,22 +1075,22 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.01507408985278991</v>
+        <v>0.0154191442103393</v>
       </c>
       <c r="C16">
-        <v>8.756130825977733e-05</v>
+        <v>8.625741441517603e-05</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16">
-        <v>0.07180355524707223</v>
+        <v>0.07193246160778481</v>
       </c>
       <c r="F16">
-        <v>1.904756250087694e-05</v>
+        <v>1.970795649484095e-05</v>
       </c>
       <c r="G16">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1098,16 +1098,16 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.6331036117460385</v>
+        <v>0.6289289442620882</v>
       </c>
       <c r="C17">
-        <v>0.02253022597692874</v>
+        <v>0.02257711703465563</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
-        <v>-0.2910644082531336</v>
+        <v>-0.2917164537828849</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1118,19 +1118,19 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>0.5735981907644438</v>
+        <v>0.5718362588075117</v>
       </c>
       <c r="C18">
-        <v>3.166160916184296e-05</v>
+        <v>2.942787591688427e-05</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>0.05061166746535808</v>
+        <v>0.05126367801504106</v>
       </c>
       <c r="G18">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1138,19 +1138,19 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>0.5065526701018932</v>
+        <v>0.5070014533863239</v>
       </c>
       <c r="C19">
-        <v>0.06860982510306927</v>
+        <v>0.07449294280185652</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
-        <v>-0.0381919377760534</v>
+        <v>-0.03739801796587516</v>
       </c>
       <c r="G19">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1158,19 +1158,19 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.544500421532061</v>
+        <v>0.5438817976461028</v>
       </c>
       <c r="C20">
-        <v>2.255545430196448e-07</v>
+        <v>2.274383424515859e-07</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20">
-        <v>0.1916525439586119</v>
+        <v>0.1912326424784251</v>
       </c>
       <c r="G20">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1178,19 +1178,19 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>0.08988515442098421</v>
+        <v>0.0857129663168017</v>
       </c>
       <c r="C21">
-        <v>3.567862672783574e-08</v>
+        <v>3.804198092776057e-08</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21">
-        <v>0.2642348546385883</v>
+        <v>0.263276559203986</v>
       </c>
       <c r="G21">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1198,19 +1198,19 @@
         <v>26</v>
       </c>
       <c r="B22">
-        <v>0.5191594322680961</v>
+        <v>0.5183929012559103</v>
       </c>
       <c r="C22">
-        <v>8.692329442561607e-13</v>
+        <v>9.410492289389598e-13</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>-0.1622512273308155</v>
+        <v>-0.1622749284403746</v>
       </c>
       <c r="G22">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1218,19 +1218,19 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>0.5484073501776345</v>
+        <v>0.5494660522501835</v>
       </c>
       <c r="C23">
-        <v>0.09716442305056736</v>
+        <v>0.09212827477338971</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23">
-        <v>0.04273533354193414</v>
+        <v>0.0434640183516067</v>
       </c>
       <c r="G23">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1238,19 +1238,19 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>0.5265285386948229</v>
+        <v>0.5252485086395167</v>
       </c>
       <c r="C24">
-        <v>0.199068479701755</v>
+        <v>0.2004523847363142</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>0.01613356418247049</v>
+        <v>0.01585134787111041</v>
       </c>
       <c r="G24">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1258,19 +1258,19 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>0.002337297925714354</v>
+        <v>0.008527629433940476</v>
       </c>
       <c r="C25">
-        <v>0.001166070092068218</v>
+        <v>0.001150911564865251</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>0.0721187304989445</v>
+        <v>0.07224775520821639</v>
       </c>
       <c r="G25">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1278,16 +1278,16 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>0.5153662676108324</v>
+        <v>0.5158091778870282</v>
       </c>
       <c r="C26">
-        <v>0.01311406613883007</v>
+        <v>0.01293695005290448</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>0.05160140275519655</v>
+        <v>0.05126542026085663</v>
       </c>
       <c r="G26">
         <v>30</v>
@@ -1298,19 +1298,19 @@
         <v>31</v>
       </c>
       <c r="B27">
-        <v>0.1241388513436668</v>
+        <v>0.1107022390139971</v>
       </c>
       <c r="C27">
-        <v>5.146620466534812e-47</v>
+        <v>9.686699077265466e-47</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27">
-        <v>0.3143954016029363</v>
+        <v>0.3135681779885129</v>
       </c>
       <c r="G27">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1318,19 +1318,19 @@
         <v>32</v>
       </c>
       <c r="B28">
-        <v>0.04922759540809718</v>
+        <v>0.05617586269777708</v>
       </c>
       <c r="C28">
-        <v>6.609441982771891e-20</v>
+        <v>4.748840683360019e-20</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28">
-        <v>0.2057191922146624</v>
+        <v>0.2064836524497995</v>
       </c>
       <c r="G28">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1338,19 +1338,19 @@
         <v>33</v>
       </c>
       <c r="B29">
-        <v>0.5177441317772389</v>
+        <v>0.5119311278178489</v>
       </c>
       <c r="C29">
-        <v>0.04847273699608069</v>
+        <v>0.04787247518300796</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29">
-        <v>0.05160034460330178</v>
+        <v>0.05126436205764957</v>
       </c>
       <c r="G29">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1358,19 +1358,19 @@
         <v>34</v>
       </c>
       <c r="B30">
-        <v>0.1195169544584624</v>
+        <v>0.1126360795307537</v>
       </c>
       <c r="C30">
-        <v>0.06666058727090333</v>
+        <v>0.0718214046957851</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30">
-        <v>-0.06400170322700129</v>
+        <v>-0.06303708498120482</v>
       </c>
       <c r="G30">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1378,19 +1378,19 @@
         <v>35</v>
       </c>
       <c r="B31">
-        <v>0.02752527485285405</v>
+        <v>0.02776310372832547</v>
       </c>
       <c r="C31">
-        <v>4.842050177314121e-14</v>
+        <v>3.72219120934917e-14</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
-        <v>-0.1806367796362009</v>
+        <v>-0.1814052911764623</v>
       </c>
       <c r="G31">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1412,19 +1412,19 @@
         <v>37</v>
       </c>
       <c r="B33">
-        <v>0.1244190257930313</v>
+        <v>0.1239969571226158</v>
       </c>
       <c r="C33">
-        <v>1.04064646943761e-18</v>
+        <v>1.049084507500979e-18</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33">
-        <v>-0.2193230311886134</v>
+        <v>-0.219249753299836</v>
       </c>
       <c r="G33">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1432,19 +1432,19 @@
         <v>38</v>
       </c>
       <c r="B34">
-        <v>0.1441091922448496</v>
+        <v>0.1309421616242807</v>
       </c>
       <c r="C34">
-        <v>1.42916701902906e-49</v>
+        <v>2.661700265692141e-49</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34">
-        <v>0.2878833456176772</v>
+        <v>0.2872130409682969</v>
       </c>
       <c r="F34">
-        <v>2.075749724380257e-06</v>
+        <v>2.073204226336693e-06</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -1455,19 +1455,19 @@
         <v>39</v>
       </c>
       <c r="B35">
-        <v>0.1190379639650461</v>
+        <v>0.1169966811365759</v>
       </c>
       <c r="C35">
-        <v>0.02140176484057398</v>
+        <v>0.02092610094983222</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35">
-        <v>-0.06846577453690936</v>
+        <v>-0.06863825346251126</v>
       </c>
       <c r="G35">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1475,19 +1475,19 @@
         <v>40</v>
       </c>
       <c r="B36">
-        <v>0.1289588400679644</v>
+        <v>0.1277638699012273</v>
       </c>
       <c r="C36">
-        <v>0.04631130983143314</v>
+        <v>0.04506120268860975</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36">
-        <v>-0.03340695728529889</v>
+        <v>-0.033626954889761</v>
       </c>
       <c r="G36">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1495,19 +1495,19 @@
         <v>41</v>
       </c>
       <c r="B37">
-        <v>0.02826166269113539</v>
+        <v>0.03234382072543607</v>
       </c>
       <c r="C37">
-        <v>0.003243905794374486</v>
+        <v>0.003345836122740219</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37">
-        <v>-0.008396579004130576</v>
+        <v>-0.007865674760171614</v>
       </c>
       <c r="G37">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1515,19 +1515,19 @@
         <v>42</v>
       </c>
       <c r="B38">
-        <v>0.02150775066874444</v>
+        <v>0.03020077185202963</v>
       </c>
       <c r="C38">
-        <v>0.1014200905364479</v>
+        <v>0.09740227982568748</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38">
-        <v>0.05138222131239235</v>
+        <v>0.05177482954892908</v>
       </c>
       <c r="G38">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1535,19 +1535,19 @@
         <v>43</v>
       </c>
       <c r="B39">
-        <v>0.03062582234186473</v>
+        <v>0.03192442600305978</v>
       </c>
       <c r="C39">
-        <v>0.1290210141392704</v>
+        <v>0.1318107139106504</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39">
-        <v>-0.01479729047228208</v>
+        <v>-0.01457946401983798</v>
       </c>
       <c r="G39">
-        <v>84</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1555,19 +1555,19 @@
         <v>44</v>
       </c>
       <c r="B40">
-        <v>0.005633895136625489</v>
+        <v>0.007198444863714792</v>
       </c>
       <c r="C40">
-        <v>0.8359594889883026</v>
+        <v>0.8307262011765919</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40">
-        <v>0.002338347406312651</v>
+        <v>0.0024784800481439</v>
       </c>
       <c r="G40">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1575,19 +1575,19 @@
         <v>45</v>
       </c>
       <c r="B41">
-        <v>0.03624772016818922</v>
+        <v>0.02661929295014787</v>
       </c>
       <c r="C41">
-        <v>0.5261293969423599</v>
+        <v>0.5320342608158347</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>0.005738523506006826</v>
+        <v>0.005913741780785967</v>
       </c>
       <c r="G41">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1595,19 +1595,19 @@
         <v>46</v>
       </c>
       <c r="B42">
-        <v>0.02274747305143698</v>
+        <v>0.03129689018511961</v>
       </c>
       <c r="C42">
-        <v>0.113243810293367</v>
+        <v>0.1325131619051086</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>0.03621460296206019</v>
+        <v>0.03464949905831885</v>
       </c>
       <c r="G42">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1615,22 +1615,22 @@
         <v>47</v>
       </c>
       <c r="B43">
-        <v>0.03843768254451074</v>
+        <v>0.02987507974747738</v>
       </c>
       <c r="C43">
-        <v>0.006297048974994609</v>
+        <v>0.005998529434834357</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43">
-        <v>0.02521454094964929</v>
+        <v>0.02553058234569726</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1638,19 +1638,19 @@
         <v>48</v>
       </c>
       <c r="B44">
-        <v>0.02994477554336683</v>
+        <v>0.03507989485788054</v>
       </c>
       <c r="C44">
-        <v>0.009427097754429284</v>
+        <v>0.00973019607929679</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44">
-        <v>-0.08325843219806786</v>
+        <v>-0.08305853851950651</v>
       </c>
       <c r="G44">
-        <v>66</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1658,19 +1658,19 @@
         <v>49</v>
       </c>
       <c r="B45">
-        <v>0.0214342615885792</v>
+        <v>0.02088837274440669</v>
       </c>
       <c r="C45">
-        <v>0.003878876705930262</v>
+        <v>0.004044573816098141</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
       <c r="E45">
-        <v>-0.03719821013129664</v>
+        <v>-0.03693718683029053</v>
       </c>
       <c r="G45">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1678,22 +1678,22 @@
         <v>50</v>
       </c>
       <c r="B46">
-        <v>0.02195132094158248</v>
+        <v>0.01094651109596234</v>
       </c>
       <c r="C46">
-        <v>0.4947891613116122</v>
+        <v>0.489520868994629</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46">
-        <v>0.003216708561120798</v>
+        <v>0.003381852179629213</v>
       </c>
       <c r="F46">
         <v>-0</v>
       </c>
       <c r="G46">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1701,19 +1701,19 @@
         <v>51</v>
       </c>
       <c r="B47">
-        <v>0.08133123153039534</v>
+        <v>0.08636481967269138</v>
       </c>
       <c r="C47">
-        <v>1.76853550106277e-20</v>
+        <v>4.588689744435122e-20</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47">
-        <v>0.2233481796836634</v>
+        <v>0.2212906134702926</v>
       </c>
       <c r="G47">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1721,19 +1721,19 @@
         <v>52</v>
       </c>
       <c r="B48">
-        <v>0.02748325535512208</v>
+        <v>0.02243121845229235</v>
       </c>
       <c r="C48">
-        <v>5.629456506180702e-07</v>
+        <v>5.18698201496845e-07</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48">
-        <v>0.1050758830545518</v>
+        <v>0.1053928268607833</v>
       </c>
       <c r="G48">
-        <v>99</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1741,19 +1741,19 @@
         <v>53</v>
       </c>
       <c r="B49">
-        <v>0.02268220716918146</v>
+        <v>0.02794547920996227</v>
       </c>
       <c r="C49">
-        <v>4.842050177307584e-14</v>
+        <v>3.722191209345837e-14</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49">
-        <v>0.1806367796362009</v>
+        <v>0.1814052911764623</v>
       </c>
       <c r="G49">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1761,19 +1761,19 @@
         <v>54</v>
       </c>
       <c r="B50">
-        <v>0.01245791614857827</v>
+        <v>0.007655789530691903</v>
       </c>
       <c r="C50">
-        <v>0.5185531549387725</v>
+        <v>0.5131497348819919</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50">
-        <v>0.03114286255904238</v>
+        <v>0.03131274115026628</v>
       </c>
       <c r="G50">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1781,19 +1781,19 @@
         <v>55</v>
       </c>
       <c r="B51">
-        <v>0.5661609312204652</v>
+        <v>0.5655682204244981</v>
       </c>
       <c r="C51">
-        <v>4.808134561005882e-30</v>
+        <v>1.007512190844525e-29</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
       <c r="E51">
-        <v>0.2685375208286064</v>
+        <v>0.2673395661147749</v>
       </c>
       <c r="G51">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1801,19 +1801,19 @@
         <v>56</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>0.002208903003243057</v>
       </c>
       <c r="C52">
-        <v>1.495783960748235e-05</v>
+        <v>1.478320224006029e-05</v>
       </c>
       <c r="D52">
         <v>1</v>
       </c>
       <c r="E52">
-        <v>0.03949120325798979</v>
+        <v>0.03953459455942442</v>
       </c>
       <c r="G52">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1821,19 +1821,19 @@
         <v>57</v>
       </c>
       <c r="B53">
-        <v>0.05142357583261337</v>
+        <v>0.05670806067141299</v>
       </c>
       <c r="C53">
-        <v>8.979177074153227e-33</v>
+        <v>1.108824864466957e-32</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53">
-        <v>-0.2437794715818961</v>
+        <v>-0.2434919805736266</v>
       </c>
       <c r="G53">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1841,19 +1841,19 @@
         <v>58</v>
       </c>
       <c r="B54">
-        <v>0.1112846011584752</v>
+        <v>0.1138238859155265</v>
       </c>
       <c r="C54">
-        <v>5.655348386616426e-15</v>
+        <v>7.354158773434474e-15</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54">
-        <v>-0.2024360170881563</v>
+        <v>-0.2017754684827343</v>
       </c>
       <c r="G54">
-        <v>68</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1861,19 +1861,19 @@
         <v>59</v>
       </c>
       <c r="B55">
-        <v>0.002535241720931669</v>
+        <v>0</v>
       </c>
       <c r="C55">
-        <v>0.0017905627672579</v>
+        <v>0.001781777413133052</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55">
-        <v>0.03422967603705188</v>
+        <v>0.03425501598655731</v>
       </c>
       <c r="G55">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1881,19 +1881,19 @@
         <v>60</v>
       </c>
       <c r="B56">
-        <v>0.08397941823873967</v>
+        <v>0.08173245278591157</v>
       </c>
       <c r="C56">
-        <v>2.65241539014671e-18</v>
+        <v>2.154360263269421e-18</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56">
-        <v>0.2329024766460886</v>
+        <v>0.233393242900475</v>
       </c>
       <c r="G56">
-        <v>92</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1901,19 +1901,19 @@
         <v>61</v>
       </c>
       <c r="B57">
-        <v>0.0120020250237729</v>
+        <v>0.01318751826953668</v>
       </c>
       <c r="C57">
-        <v>3.756899082824071e-14</v>
+        <v>3.689746055814635e-14</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57">
-        <v>0.09687998078683717</v>
+        <v>0.09691681560318771</v>
       </c>
       <c r="G57">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1921,19 +1921,19 @@
         <v>62</v>
       </c>
       <c r="B58">
-        <v>0.03632313168152534</v>
+        <v>0.03805990204150667</v>
       </c>
       <c r="C58">
-        <v>7.03243346378324e-19</v>
+        <v>2.168974205138719e-18</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58">
-        <v>0.2152981304035025</v>
+        <v>0.2127679000620672</v>
       </c>
       <c r="G58">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1941,19 +1941,19 @@
         <v>63</v>
       </c>
       <c r="B59">
-        <v>0.0358567059805619</v>
+        <v>0.0407022396395964</v>
       </c>
       <c r="C59">
-        <v>1.768980404216941e-09</v>
+        <v>2.201933518769281e-09</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59">
-        <v>-0.141655891826069</v>
+        <v>-0.14093467028545</v>
       </c>
       <c r="G59">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -1961,19 +1961,19 @@
         <v>64</v>
       </c>
       <c r="B60">
-        <v>0.1018115970049109</v>
+        <v>0.1016809577371061</v>
       </c>
       <c r="C60">
-        <v>3.170260343999953e-20</v>
+        <v>4.690834057684993e-20</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
       <c r="E60">
-        <v>-0.2281575418637311</v>
+        <v>-0.2273313500451997</v>
       </c>
       <c r="G60">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1981,19 +1981,19 @@
         <v>65</v>
       </c>
       <c r="B61">
-        <v>0.0392046242664561</v>
+        <v>0.03913243249766318</v>
       </c>
       <c r="C61">
-        <v>4.727036644430333e-06</v>
+        <v>4.395336093265152e-06</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
       <c r="E61">
-        <v>0.1161390257150837</v>
+        <v>0.116456168982002</v>
       </c>
       <c r="G61">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2001,19 +2001,19 @@
         <v>66</v>
       </c>
       <c r="B62">
-        <v>0.06311249988749412</v>
+        <v>0.06261528034678387</v>
       </c>
       <c r="C62">
-        <v>4.5250820298812e-21</v>
+        <v>1.043651976371202e-20</v>
       </c>
       <c r="D62">
         <v>1</v>
       </c>
       <c r="E62">
-        <v>0.2400017870770367</v>
+        <v>0.2382498208503458</v>
       </c>
       <c r="G62">
-        <v>97</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2021,19 +2021,19 @@
         <v>67</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>0.007500086933217354</v>
       </c>
       <c r="C63">
-        <v>2.701326995697757e-08</v>
+        <v>2.690458255867819e-08</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63">
-        <v>0.04082367304930539</v>
+        <v>0.04082997349243986</v>
       </c>
       <c r="G63">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2041,19 +2041,19 @@
         <v>68</v>
       </c>
       <c r="B64">
-        <v>0.01138139674814775</v>
+        <v>0.007818433596551877</v>
       </c>
       <c r="C64">
-        <v>0.0001663334620063759</v>
+        <v>0.0001636993873578531</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64">
-        <v>0.08654070825025262</v>
+        <v>0.08662175991821815</v>
       </c>
       <c r="G64">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2061,19 +2061,19 @@
         <v>69</v>
       </c>
       <c r="B65">
-        <v>0.1670367726257176</v>
+        <v>0.1690207205962773</v>
       </c>
       <c r="C65">
-        <v>7.138670933588294e-52</v>
+        <v>1.429044615013101e-51</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65">
-        <v>-0.3620908121492698</v>
+        <v>-0.3612322346078113</v>
       </c>
       <c r="G65">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2081,19 +2081,19 @@
         <v>70</v>
       </c>
       <c r="B66">
-        <v>0.02646387509791714</v>
+        <v>0.03191732814256798</v>
       </c>
       <c r="C66">
-        <v>0.02247423576650534</v>
+        <v>0.02144060541739326</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="E66">
-        <v>0.07281541213094908</v>
+        <v>0.07317354138392185</v>
       </c>
       <c r="G66">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2101,19 +2101,19 @@
         <v>71</v>
       </c>
       <c r="B67">
-        <v>0.1221192764302148</v>
+        <v>0.1141026636922058</v>
       </c>
       <c r="C67">
-        <v>1.44204257237566e-49</v>
+        <v>3.990447783327807e-49</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67">
-        <v>0.3393042724155369</v>
+        <v>0.338003921004937</v>
       </c>
       <c r="G67">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2121,19 +2121,19 @@
         <v>72</v>
       </c>
       <c r="B68">
-        <v>0.08765905629781212</v>
+        <v>0.0788844527398449</v>
       </c>
       <c r="C68">
-        <v>2.932563118973882e-31</v>
+        <v>5.60366388572047e-31</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="E68">
-        <v>0.2749495540669539</v>
+        <v>0.2738905992280676</v>
       </c>
       <c r="G68">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2141,19 +2141,19 @@
         <v>73</v>
       </c>
       <c r="B69">
-        <v>0.04410338079793541</v>
+        <v>0.03359123962432831</v>
       </c>
       <c r="C69">
-        <v>2.399855631295514e-06</v>
+        <v>2.849351032326759e-06</v>
       </c>
       <c r="D69">
         <v>1</v>
       </c>
       <c r="E69">
-        <v>0.1235491342361309</v>
+        <v>0.1228337069101701</v>
       </c>
       <c r="G69">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2161,19 +2161,19 @@
         <v>74</v>
       </c>
       <c r="B70">
-        <v>0.001762729859010825</v>
+        <v>0.001625605853352585</v>
       </c>
       <c r="C70">
-        <v>7.406647137362754e-05</v>
+        <v>7.278244508487633e-05</v>
       </c>
       <c r="D70">
         <v>1</v>
       </c>
       <c r="E70">
-        <v>0.07150626578226432</v>
+        <v>0.07158556876563407</v>
       </c>
       <c r="G70">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2181,16 +2181,16 @@
         <v>75</v>
       </c>
       <c r="B71">
-        <v>0.5201668346391886</v>
+        <v>0.5222171965074063</v>
       </c>
       <c r="C71">
-        <v>1.267131174465186e-09</v>
+        <v>2.322728760901401e-09</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71">
-        <v>0.123831555355631</v>
+        <v>0.1226055883417212</v>
       </c>
       <c r="G71">
         <v>28</v>
@@ -2201,19 +2201,19 @@
         <v>76</v>
       </c>
       <c r="B72">
-        <v>0.592554000810706</v>
+        <v>0.5896504468989026</v>
       </c>
       <c r="C72">
-        <v>3.495464518594867e-25</v>
+        <v>8.45766918322308e-25</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
       <c r="E72">
-        <v>0.2975835158912593</v>
+        <v>0.2964252283225013</v>
       </c>
       <c r="G72">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2221,19 +2221,19 @@
         <v>77</v>
       </c>
       <c r="B73">
-        <v>0.04942637388686477</v>
+        <v>0.05960293582873044</v>
       </c>
       <c r="C73">
-        <v>5.069887697963868e-13</v>
+        <v>5.697884349048242e-13</v>
       </c>
       <c r="D73">
         <v>1</v>
       </c>
       <c r="E73">
-        <v>-0.142082705449536</v>
+        <v>-0.1417805156443175</v>
       </c>
       <c r="G73">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2241,19 +2241,19 @@
         <v>78</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>0.002310867324815113</v>
       </c>
       <c r="C74">
-        <v>6.183587647228256e-09</v>
+        <v>6.06227109224784e-09</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
       <c r="E74">
-        <v>0.06670915961658888</v>
+        <v>0.06677259347728386</v>
       </c>
       <c r="G74">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2261,19 +2261,19 @@
         <v>79</v>
       </c>
       <c r="B75">
-        <v>0.1080880988527984</v>
+        <v>0.1127133924909434</v>
       </c>
       <c r="C75">
-        <v>3.697177345126928e-23</v>
+        <v>5.721589015612057e-23</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75">
-        <v>0.2336822722855303</v>
+        <v>0.2328330536196253</v>
       </c>
       <c r="G75">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2281,22 +2281,22 @@
         <v>80</v>
       </c>
       <c r="B76">
-        <v>0.04761595455154422</v>
+        <v>0.03410822156366855</v>
       </c>
       <c r="C76">
-        <v>0.468295538271831</v>
+        <v>0.4532140687401</v>
       </c>
       <c r="D76">
         <v>0</v>
       </c>
       <c r="E76">
-        <v>0.0145853125827676</v>
+        <v>0.01508105357508985</v>
       </c>
       <c r="F76">
         <v>0</v>
       </c>
       <c r="G76">
-        <v>86</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2304,22 +2304,22 @@
         <v>81</v>
       </c>
       <c r="B77">
-        <v>0.01167646998970473</v>
+        <v>0.02865092606703623</v>
       </c>
       <c r="C77">
-        <v>0.02608557889945307</v>
+        <v>0.02529005608539448</v>
       </c>
       <c r="D77">
         <v>1</v>
       </c>
       <c r="E77">
-        <v>0.0508664241454088</v>
+        <v>0.05110581784530612</v>
       </c>
       <c r="F77">
         <v>-0</v>
       </c>
       <c r="G77">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2327,22 +2327,22 @@
         <v>82</v>
       </c>
       <c r="B78">
-        <v>0.04241637753731586</v>
+        <v>0.04604367020065259</v>
       </c>
       <c r="C78">
-        <v>8.109589003510044e-15</v>
+        <v>1.640372374695625e-14</v>
       </c>
       <c r="D78">
         <v>1</v>
       </c>
       <c r="E78">
-        <v>0.172534127951163</v>
+        <v>0.1707654558064993</v>
       </c>
       <c r="F78">
         <v>0</v>
       </c>
       <c r="G78">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2350,19 +2350,19 @@
         <v>83</v>
       </c>
       <c r="B79">
-        <v>0.04674902926724722</v>
+        <v>0.04864946930222636</v>
       </c>
       <c r="C79">
-        <v>0.001872880076807394</v>
+        <v>0.002035901997645596</v>
       </c>
       <c r="D79">
         <v>1</v>
       </c>
       <c r="E79">
-        <v>-0.08663028888747817</v>
+        <v>-0.08613863237295494</v>
       </c>
       <c r="G79">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2370,19 +2370,19 @@
         <v>84</v>
       </c>
       <c r="B80">
-        <v>0.08110249612236231</v>
+        <v>0.0699699594833032</v>
       </c>
       <c r="C80">
-        <v>1.673623582349678e-16</v>
+        <v>2.494283196300772e-16</v>
       </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="E80">
-        <v>0.2056459268063707</v>
+        <v>0.2047135543847723</v>
       </c>
       <c r="G80">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2390,19 +2390,19 @@
         <v>85</v>
       </c>
       <c r="B81">
-        <v>0.01729688340963942</v>
+        <v>0.01835273388716496</v>
       </c>
       <c r="C81">
-        <v>3.49841610996925e-11</v>
+        <v>3.408610874911918e-11</v>
       </c>
       <c r="D81">
         <v>1</v>
       </c>
       <c r="E81">
-        <v>0.1032310249200499</v>
+        <v>0.1032982999216141</v>
       </c>
       <c r="G81">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2410,19 +2410,19 @@
         <v>86</v>
       </c>
       <c r="B82">
-        <v>0.09788470566071772</v>
+        <v>0.1063300535500173</v>
       </c>
       <c r="C82">
-        <v>1.48946759523581e-39</v>
+        <v>2.618036899586744e-39</v>
       </c>
       <c r="D82">
         <v>1</v>
       </c>
       <c r="E82">
-        <v>-0.2924559194379514</v>
+        <v>-0.2916419300705876</v>
       </c>
       <c r="G82">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2430,19 +2430,19 @@
         <v>87</v>
       </c>
       <c r="B83">
-        <v>0.03591707526310217</v>
+        <v>0.02808530602325443</v>
       </c>
       <c r="C83">
-        <v>0.01549906342703994</v>
+        <v>0.0147847693742874</v>
       </c>
       <c r="D83">
         <v>1</v>
       </c>
       <c r="E83">
-        <v>0.04812907624357016</v>
+        <v>0.04846483945148854</v>
       </c>
       <c r="G83">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2450,19 +2450,19 @@
         <v>88</v>
       </c>
       <c r="B84">
-        <v>0.06831911524416578</v>
+        <v>0.08268443314090357</v>
       </c>
       <c r="C84">
-        <v>2.056582129762175e-32</v>
+        <v>4.24661393218465e-32</v>
       </c>
       <c r="D84">
         <v>1</v>
       </c>
       <c r="E84">
-        <v>0.27149652657144</v>
+        <v>0.2703316185847989</v>
       </c>
       <c r="G84">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2470,19 +2470,19 @@
         <v>89</v>
       </c>
       <c r="B85">
-        <v>0.0731668239339982</v>
+        <v>0.08002046475184987</v>
       </c>
       <c r="C85">
-        <v>4.454370337109773e-21</v>
+        <v>5.769540416039289e-21</v>
       </c>
       <c r="D85">
         <v>1</v>
       </c>
       <c r="E85">
-        <v>-0.2037050582884197</v>
+        <v>-0.203178838308448</v>
       </c>
       <c r="G85">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2490,19 +2490,19 @@
         <v>90</v>
       </c>
       <c r="B86">
-        <v>0.1020187791190914</v>
+        <v>0.1003741962880429</v>
       </c>
       <c r="C86">
-        <v>1.998773608553395e-31</v>
+        <v>3.130610728343713e-31</v>
       </c>
       <c r="D86">
         <v>1</v>
       </c>
       <c r="E86">
-        <v>0.2574653127177628</v>
+        <v>0.2567318651683397</v>
       </c>
       <c r="G86">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2510,19 +2510,19 @@
         <v>91</v>
       </c>
       <c r="B87">
-        <v>0.009933712126751537</v>
+        <v>0.006403240895322737</v>
       </c>
       <c r="C87">
-        <v>0.2091429542135475</v>
+        <v>0.207002473962135</v>
       </c>
       <c r="D87">
         <v>0</v>
       </c>
       <c r="E87">
-        <v>0.03639783143046825</v>
+        <v>0.03652028987864669</v>
       </c>
       <c r="G87">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2530,19 +2530,19 @@
         <v>92</v>
       </c>
       <c r="B88">
-        <v>0.01542919515560159</v>
+        <v>0.0007686838065095181</v>
       </c>
       <c r="C88">
-        <v>1.469774463409074e-05</v>
+        <v>1.454250643119292e-05</v>
       </c>
       <c r="D88">
         <v>1</v>
       </c>
       <c r="E88">
-        <v>0.09436816222404697</v>
+        <v>0.09440963021858445</v>
       </c>
       <c r="G88">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2550,19 +2550,19 @@
         <v>93</v>
       </c>
       <c r="B89">
-        <v>0.06688497911144275</v>
+        <v>0.0618770432222322</v>
       </c>
       <c r="C89">
-        <v>4.314291115377936e-26</v>
+        <v>2.593344449943603e-26</v>
       </c>
       <c r="D89">
         <v>1</v>
       </c>
       <c r="E89">
-        <v>-0.2184132199574969</v>
+        <v>-0.2194104431814166</v>
       </c>
       <c r="G89">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2570,19 +2570,19 @@
         <v>94</v>
       </c>
       <c r="B90">
-        <v>0.5740132768118986</v>
+        <v>0.5722791983923328</v>
       </c>
       <c r="C90">
-        <v>3.492518110022227e-05</v>
+        <v>3.246312212120736e-05</v>
       </c>
       <c r="D90">
         <v>1</v>
       </c>
       <c r="E90">
-        <v>0.05061162041649789</v>
+        <v>0.05126363091888878</v>
       </c>
       <c r="G90">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2590,19 +2590,19 @@
         <v>95</v>
       </c>
       <c r="B91">
-        <v>0.4959234590940431</v>
+        <v>0.4967812969180043</v>
       </c>
       <c r="C91">
-        <v>0.2493210396742308</v>
+        <v>0.2641557358446532</v>
       </c>
       <c r="D91">
         <v>0</v>
       </c>
       <c r="E91">
-        <v>-0.0381919377760534</v>
+        <v>-0.03739801796587516</v>
       </c>
       <c r="G91">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2610,19 +2610,19 @@
         <v>96</v>
       </c>
       <c r="B92">
-        <v>0.5311440840566117</v>
+        <v>0.528493594605763</v>
       </c>
       <c r="C92">
-        <v>0.00428036442591581</v>
+        <v>0.004133756432852777</v>
       </c>
       <c r="D92">
         <v>1</v>
       </c>
       <c r="E92">
-        <v>0.1916525439586119</v>
+        <v>0.1912326424784251</v>
       </c>
       <c r="G92">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2630,19 +2630,19 @@
         <v>97</v>
       </c>
       <c r="B93">
-        <v>0.09146664594333442</v>
+        <v>0.09552613743068683</v>
       </c>
       <c r="C93">
-        <v>5.565074857662266e-18</v>
+        <v>7.632780424449975e-18</v>
       </c>
       <c r="D93">
         <v>1</v>
       </c>
       <c r="E93">
-        <v>0.2642348546385883</v>
+        <v>0.263276559203986</v>
       </c>
       <c r="G93">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2650,19 +2650,19 @@
         <v>98</v>
       </c>
       <c r="B94">
-        <v>0.523709931893988</v>
+        <v>0.5214184338538805</v>
       </c>
       <c r="C94">
-        <v>1.118330110527993e-12</v>
+        <v>1.21022472910516e-12</v>
       </c>
       <c r="D94">
         <v>1</v>
       </c>
       <c r="E94">
-        <v>-0.1622508926675772</v>
+        <v>-0.162274593823075</v>
       </c>
       <c r="G94">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2670,19 +2670,19 @@
         <v>99</v>
       </c>
       <c r="B95">
-        <v>0.529345602757795</v>
+        <v>0.5273312992329195</v>
       </c>
       <c r="C95">
-        <v>0.641588954118509</v>
+        <v>0.6384150952997548</v>
       </c>
       <c r="D95">
         <v>0</v>
       </c>
       <c r="E95">
-        <v>0.01613356418247049</v>
+        <v>0.01585134787111041</v>
       </c>
       <c r="G95">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2690,16 +2690,16 @@
         <v>100</v>
       </c>
       <c r="B96">
-        <v>0.01630877538941267</v>
+        <v>0.008214060754768715</v>
       </c>
       <c r="C96">
-        <v>0.00411610293375642</v>
+        <v>0.004033147066663031</v>
       </c>
       <c r="D96">
         <v>1</v>
       </c>
       <c r="E96">
-        <v>0.07120322740120207</v>
+        <v>0.07133232594520077</v>
       </c>
       <c r="G96">
         <v>80</v>
@@ -2710,19 +2710,19 @@
         <v>101</v>
       </c>
       <c r="B97">
-        <v>0.06234333204140974</v>
+        <v>0.06480149530923685</v>
       </c>
       <c r="C97">
-        <v>0.008260954735493016</v>
+        <v>0.008259022829519997</v>
       </c>
       <c r="D97">
         <v>1</v>
       </c>
       <c r="E97">
-        <v>-0.04949605690183231</v>
+        <v>-0.04972064982617809</v>
       </c>
       <c r="G97">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2730,19 +2730,19 @@
         <v>102</v>
       </c>
       <c r="B98">
-        <v>0.04903815463430772</v>
+        <v>0.05257783103663072</v>
       </c>
       <c r="C98">
-        <v>6.609441982771891e-20</v>
+        <v>4.748840683360019e-20</v>
       </c>
       <c r="D98">
         <v>1</v>
       </c>
       <c r="E98">
-        <v>0.2057191922146624</v>
+        <v>0.2064836524497995</v>
       </c>
       <c r="G98">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2750,16 +2750,16 @@
         <v>103</v>
       </c>
       <c r="B99">
-        <v>1.012573424816218</v>
+        <v>1.007860400507876</v>
       </c>
       <c r="C99">
-        <v>5.678095347169994e-85</v>
+        <v>1.304039872553797e-84</v>
       </c>
       <c r="D99">
         <v>1</v>
       </c>
       <c r="E99">
-        <v>0.5213783676916479</v>
+        <v>0.520405011970143</v>
       </c>
       <c r="G99">
         <v>1</v>
@@ -2770,16 +2770,16 @@
         <v>104</v>
       </c>
       <c r="B100">
-        <v>0.8253980873350724</v>
+        <v>0.8255730988069807</v>
       </c>
       <c r="C100">
-        <v>9.689501633735791e-126</v>
+        <v>2.473770149832947e-125</v>
       </c>
       <c r="D100">
         <v>1</v>
       </c>
       <c r="E100">
-        <v>0.5276784377081657</v>
+        <v>0.5268272427731665</v>
       </c>
       <c r="G100">
         <v>1</v>
@@ -2790,16 +2790,16 @@
         <v>105</v>
       </c>
       <c r="B101">
-        <v>0.572399795250722</v>
+        <v>0.5700492920194096</v>
       </c>
       <c r="C101">
-        <v>0.002635843584817047</v>
+        <v>0.002597415595167928</v>
       </c>
       <c r="D101">
         <v>1</v>
       </c>
       <c r="E101">
-        <v>-0.2515850255379993</v>
+        <v>-0.2526042382118892</v>
       </c>
       <c r="G101">
         <v>1</v>
@@ -2810,16 +2810,16 @@
         <v>106</v>
       </c>
       <c r="B102">
-        <v>0.5162407654219736</v>
+        <v>0.5184285848756378</v>
       </c>
       <c r="C102">
-        <v>7.511718488100377e-05</v>
+        <v>6.833542102838046e-05</v>
       </c>
       <c r="D102">
         <v>1</v>
       </c>
       <c r="E102">
-        <v>0.04587308952425403</v>
+        <v>0.0468111452743698</v>
       </c>
       <c r="G102">
         <v>25</v>
@@ -2830,16 +2830,16 @@
         <v>107</v>
       </c>
       <c r="B103">
-        <v>0.5174960731960532</v>
+        <v>0.5171147848825912</v>
       </c>
       <c r="C103">
-        <v>0.1039395411577813</v>
+        <v>0.1124356163470952</v>
       </c>
       <c r="D103">
         <v>0</v>
       </c>
       <c r="E103">
-        <v>-0.03287533253219302</v>
+        <v>-0.03205651056149528</v>
       </c>
       <c r="G103">
         <v>12</v>
@@ -2850,19 +2850,19 @@
         <v>108</v>
       </c>
       <c r="B104">
-        <v>0.5451079259151941</v>
+        <v>0.5442969566509124</v>
       </c>
       <c r="C104">
-        <v>1.221325345924656e-07</v>
+        <v>1.225795984642769e-07</v>
       </c>
       <c r="D104">
         <v>1</v>
       </c>
       <c r="E104">
-        <v>0.191303069789983</v>
+        <v>0.1908930927238916</v>
       </c>
       <c r="G104">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -2870,19 +2870,19 @@
         <v>109</v>
       </c>
       <c r="B105">
-        <v>0.5086736305134414</v>
+        <v>0.5051275430950053</v>
       </c>
       <c r="C105">
-        <v>4.415738571622948e-13</v>
+        <v>4.847029183635016e-13</v>
       </c>
       <c r="D105">
         <v>1</v>
       </c>
       <c r="E105">
-        <v>-0.1654653837824865</v>
+        <v>-0.1654476527606736</v>
       </c>
       <c r="G105">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -2890,16 +2890,16 @@
         <v>110</v>
       </c>
       <c r="B106">
-        <v>0.5176073963276719</v>
+        <v>0.5168284404275969</v>
       </c>
       <c r="C106">
-        <v>0.3395698785407533</v>
+        <v>0.3267825622668317</v>
       </c>
       <c r="D106">
         <v>0</v>
       </c>
       <c r="E106">
-        <v>0.0380147777728414</v>
+        <v>0.03877247512178312</v>
       </c>
       <c r="G106">
         <v>35</v>
@@ -2910,19 +2910,19 @@
         <v>111</v>
       </c>
       <c r="B107">
-        <v>0.5121767138270803</v>
+        <v>0.5132883189239488</v>
       </c>
       <c r="C107">
-        <v>0.5801377439252333</v>
+        <v>0.5801018888066414</v>
       </c>
       <c r="D107">
         <v>0</v>
       </c>
       <c r="E107">
-        <v>0.012030525654625</v>
+        <v>0.01167689255912605</v>
       </c>
       <c r="G107">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -2930,16 +2930,16 @@
         <v>112</v>
       </c>
       <c r="B108">
-        <v>0.5303111127260189</v>
+        <v>0.5322819875273277</v>
       </c>
       <c r="C108">
-        <v>0.0001346262431981488</v>
+        <v>0.0001236165529516998</v>
       </c>
       <c r="D108">
         <v>1</v>
       </c>
       <c r="E108">
-        <v>0.03933925002286111</v>
+        <v>0.04023389559030272</v>
       </c>
       <c r="G108">
         <v>7</v>
@@ -2950,19 +2950,19 @@
         <v>113</v>
       </c>
       <c r="B109">
-        <v>0.5085315672424908</v>
+        <v>0.5086691882850056</v>
       </c>
       <c r="C109">
-        <v>0.1943095366110579</v>
+        <v>0.2069335283959722</v>
       </c>
       <c r="D109">
         <v>0</v>
       </c>
       <c r="E109">
-        <v>-0.02881114750724708</v>
+        <v>-0.02804677022726094</v>
       </c>
       <c r="G109">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -2970,19 +2970,19 @@
         <v>114</v>
       </c>
       <c r="B110">
-        <v>0.5453739692742179</v>
+        <v>0.5506612816257919</v>
       </c>
       <c r="C110">
-        <v>3.931012545434587e-07</v>
+        <v>3.954721719743978e-07</v>
       </c>
       <c r="D110">
         <v>1</v>
       </c>
       <c r="E110">
-        <v>0.1919688559931708</v>
+        <v>0.1915449630086061</v>
       </c>
       <c r="G110">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -2990,19 +2990,19 @@
         <v>115</v>
       </c>
       <c r="B111">
-        <v>0.5196109505219386</v>
+        <v>0.5211007928156706</v>
       </c>
       <c r="C111">
-        <v>7.417050391756612e-13</v>
+        <v>8.060386439768152e-13</v>
       </c>
       <c r="D111">
         <v>1</v>
       </c>
       <c r="E111">
-        <v>-0.1630727026574812</v>
+        <v>-0.1630847607495906</v>
       </c>
       <c r="G111">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -3010,19 +3010,19 @@
         <v>116</v>
       </c>
       <c r="B112">
-        <v>0.5213047253400163</v>
+        <v>0.5229482615880769</v>
       </c>
       <c r="C112">
-        <v>0.3427150093432352</v>
+        <v>0.3296618384712726</v>
       </c>
       <c r="D112">
         <v>0</v>
       </c>
       <c r="E112">
-        <v>0.0384419403681563</v>
+        <v>0.03922368025655589</v>
       </c>
       <c r="G112">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -3030,19 +3030,19 @@
         <v>117</v>
       </c>
       <c r="B113">
-        <v>0.5006260658467632</v>
+        <v>0.4937128596610414</v>
       </c>
       <c r="C113">
-        <v>0.8115997121384951</v>
+        <v>0.812166499230918</v>
       </c>
       <c r="D113">
         <v>0</v>
       </c>
       <c r="E113">
-        <v>0.02143062444207226</v>
+        <v>0.02112501133246244</v>
       </c>
       <c r="G113">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>